<commit_message>
fix: Novas Cores de cabeçalhos
</commit_message>
<xml_diff>
--- a/Planilha_Financeira.xlsx
+++ b/Planilha_Financeira.xlsx
@@ -133,12 +133,17 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFADD8E6"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -148,6 +153,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF08080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8C00"/>
       </patternFill>
     </fill>
   </fills>
@@ -163,13 +173,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" applyFill="1"/>
     <xf numFmtId="2" applyNumberFormat="1" fontId="0" xfId="0"/>
     <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="2" applyFill="1"/>
     <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="3" applyFill="1"/>
+    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" applyFill="1"/>
+    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="5" applyFill="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -190,16 +204,18 @@
     <col min="1" max="1" width="37.10316848754883" customWidth="1"/>
     <col min="2" max="2" width="29.43222427368164" customWidth="1"/>
     <col min="3" max="3" width="14.456594467163086" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1" style="3"/>
+    <col min="4" max="4" width="9.140625" customWidth="1" style="4"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
@@ -207,16 +223,16 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -230,7 +246,7 @@
       <c r="C6" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="4">
         <v>1500</v>
       </c>
     </row>
@@ -244,7 +260,7 @@
       <c r="C7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="4">
         <v>5000</v>
       </c>
     </row>
@@ -258,7 +274,7 @@
       <c r="C8" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="4">
         <v>2500</v>
       </c>
     </row>
@@ -272,7 +288,7 @@
       <c r="C9" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="4">
         <v>3500</v>
       </c>
     </row>
@@ -286,7 +302,7 @@
       <c r="C10" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="4">
         <v>1200</v>
       </c>
     </row>
@@ -296,16 +312,16 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -319,7 +335,7 @@
       <c r="C14" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="4">
         <v>3000</v>
       </c>
     </row>
@@ -333,7 +349,7 @@
       <c r="C15" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="4">
         <v>1200</v>
       </c>
     </row>
@@ -347,7 +363,7 @@
       <c r="C16" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="4">
         <v>2000</v>
       </c>
     </row>
@@ -361,20 +377,23 @@
       <c r="C17" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="4">
         <v>1600</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="8" t="s">
         <v>32</v>
       </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9"/>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="4">
         <f>SUM(D6:D10)</f>
       </c>
     </row>
@@ -382,7 +401,7 @@
       <c r="A21" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="4">
         <f>SUM(D14:D17)</f>
       </c>
     </row>
@@ -390,7 +409,7 @@
       <c r="A22" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="4">
         <f>B20 - B21</f>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: ajuste de saldo
</commit_message>
<xml_diff>
--- a/Planilha_Financeira.xlsx
+++ b/Planilha_Financeira.xlsx
@@ -20,7 +20,7 @@
     <t>Período Financeiro: Janeiro 2024</t>
   </si>
   <si>
-    <t>Receitas</t>
+    <t>RECEITAS</t>
   </si>
   <si>
     <t>Data</t>
@@ -32,7 +32,7 @@
     <t>Categoria</t>
   </si>
   <si>
-    <t>Valor</t>
+    <t>Valor (BRL)</t>
   </si>
   <si>
     <t>11/01/2024</t>
@@ -80,7 +80,7 @@
     <t>Operações</t>
   </si>
   <si>
-    <t>Despesas</t>
+    <t>DESPESAS</t>
   </si>
   <si>
     <t>02/01/2024</t>
@@ -126,7 +126,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="R$ #,##0.00"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -178,12 +180,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" applyFill="1"/>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" xfId="0"/>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="2" applyFill="1"/>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="3" applyFill="1"/>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="4" applyFill="1"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" xfId="0"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" fillId="2" applyFill="1"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" fillId="3" applyFill="1"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" fillId="4" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" applyFill="1"/>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="5" applyFill="1" xfId="0"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" fillId="5" applyFill="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -204,7 +206,7 @@
     <col min="1" max="1" width="37.10316848754883" customWidth="1"/>
     <col min="2" max="2" width="29.43222427368164" customWidth="1"/>
     <col min="3" max="3" width="14.456594467163086" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1" style="4"/>
+    <col min="4" max="4" width="12.190505027770996" customWidth="1" style="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -275,7 +277,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="4">
-        <v>2500</v>
+        <v>12500</v>
       </c>
     </row>
     <row r="9">
@@ -303,7 +305,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="4">
-        <v>1200</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="12">
@@ -364,7 +366,7 @@
         <v>30</v>
       </c>
       <c r="D16" s="4">
-        <v>2000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="17">
@@ -378,7 +380,7 @@
         <v>15</v>
       </c>
       <c r="D17" s="4">
-        <v>1600</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="19">
@@ -410,7 +412,7 @@
         <v>35</v>
       </c>
       <c r="D22" s="4">
-        <f>B20 - B21</f>
+        <f>D20 - D21</f>
       </c>
     </row>
   </sheetData>

</xml_diff>